<commit_message>
Added formulas to Normal_Bell_Curve.xlsx
</commit_message>
<xml_diff>
--- a/Formulas_and_Templates/Templates/Normal_Bell_Curve/Normal_Bell_Curve.xlsx
+++ b/Formulas_and_Templates/Templates/Normal_Bell_Curve/Normal_Bell_Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\DADS\GitHub_Repositories\Excel\Formulas_and_Templates\Templates\Normal_Bell_Curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC1B311-3FA5-4CE3-912E-F7480D6F52FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410EE091-C86E-496C-981F-27BEC76F8EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12126" yWindow="18" windowWidth="10782" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12126" yWindow="0" windowWidth="10782" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1694,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1709,7 +1698,7 @@
     <col min="7" max="7" width="19.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1719,12 +1708,19 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="3">
+        <f>_xlfn.NORM.DIST(92,B1,B2,FALSE)</f>
+        <v>1.8413507015166166E-2</v>
+      </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1">
+        <f>_xlfn.NORM.INV(33%,B1,B2)</f>
+        <v>91.201736686535327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1734,12 +1730,19 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3">
+        <f>1-_xlfn.NORM.DIST(92,B1,B2,TRUE)</f>
+        <v>0.65542174161032429</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2">
+        <f>_xlfn.NORM.INV(1-90%,B1,B2)</f>
+        <v>74.368968689107987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>36</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>1.1920441007324202E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>38</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>1.6334095280999593E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>2.2159242059690038E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>42</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>2.9762662098879267E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>44</v>
       </c>
@@ -1784,7 +1787,7 @@
         <v>3.9577257914899847E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>46</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>5.2104674072112956E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>48</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>6.7914846168428062E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>50</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>8.7641502467842702E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>52</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>1.1197265147421451E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>54</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>1.4163518870800593E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>56</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>1.773729642311571E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>58</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>2.1991797990213598E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>60</v>
       </c>

</xml_diff>